<commit_message>
fix a formatting error in table
</commit_message>
<xml_diff>
--- a/labo1/datos_experimentales.xlsx
+++ b/labo1/datos_experimentales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\mierda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\produccion_acetato_etilo\labo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A130B-F511-4202-8DB8-7B21558CBAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387EAD85-8C26-45FB-B137-D27B85B5BD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="19200" windowHeight="7344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="19200" windowHeight="7344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -81,8 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,26 +369,29 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -398,6 +404,7 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -600,6 +607,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>